<commit_message>
It came to me in a dream.
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sirli\Documents\DA13\Excel\lookups-exercise-ryanphenderson\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885C02F9-8D37-4F6E-9515-F9A6A2FD99C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC34943D-E97A-477C-AFE6-B42CF62CE3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,18 @@
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
     <sheet name="data_dictionary" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="Department">metro_budget!$A$1:$A$52</definedName>
+    <definedName name="FY17_diff">metro_budget!$D$1:$D$52</definedName>
+    <definedName name="FY17_pct">metro_budget!$E$1:$E$52</definedName>
+    <definedName name="FY17_rank">metro_budget!$F$1:$F$52</definedName>
+    <definedName name="FY18_diff">metro_budget!$I$1:$I$52</definedName>
+    <definedName name="FY18_pct">metro_budget!$J$1:$J$52</definedName>
+    <definedName name="FY18_rank">metro_budget!$K$1:$K$52</definedName>
+    <definedName name="FY19_diff">metro_budget!$N$1:$N$52</definedName>
+    <definedName name="FY19_pct">metro_budget!$O$1:$O$52</definedName>
+    <definedName name="FY19_rank">metro_budget!$P$1:$P$52</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,6 +43,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1178,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4403,16 +4437,16 @@
       <c r="A65" t="s">
         <v>24</v>
       </c>
-      <c r="B65">
-        <f>_xlfn.XLOOKUP($A65,$A$2:$A$52,$D$2:$D$52,"N/A",0)</f>
+      <c r="B65" cm="1">
+        <f t="array" aca="1" ref="B65" ca="1">_xlfn.XLOOKUP($A65,INDIRECT($A$64),INDIRECT(B$64))</f>
         <v>-36209.630000000005</v>
       </c>
-      <c r="C65">
-        <f>_xlfn.XLOOKUP($A65,$A$2:$A$52,$I$2:$I$52,"N/A",0)</f>
+      <c r="C65" cm="1">
+        <f t="array" aca="1" ref="C65" ca="1">_xlfn.XLOOKUP($A65,INDIRECT($A$64),INDIRECT(C$64))</f>
         <v>-27292.159999999974</v>
       </c>
-      <c r="D65">
-        <f>_xlfn.XLOOKUP($A65,$A$2:$A$52,$N$2:$N$52,"N/A",0)</f>
+      <c r="D65" cm="1">
+        <f t="array" aca="1" ref="D65" ca="1">_xlfn.XLOOKUP($A65,INDIRECT($A$64),INDIRECT(D$64))</f>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -4420,16 +4454,16 @@
       <c r="A66" t="s">
         <v>25</v>
       </c>
-      <c r="B66">
-        <f t="shared" ref="B66:B70" si="13">_xlfn.XLOOKUP($A66,$A$2:$A$52,$D$2:$D$52,"N/A",0)</f>
-        <v>0</v>
-      </c>
-      <c r="C66">
-        <f t="shared" ref="C66:C70" si="14">_xlfn.XLOOKUP($A66,$A$2:$A$52,$I$2:$I$52,"N/A",0)</f>
-        <v>0</v>
-      </c>
-      <c r="D66">
-        <f t="shared" ref="D66:D70" si="15">_xlfn.XLOOKUP($A66,$A$2:$A$52,$N$2:$N$52,"N/A",0)</f>
+      <c r="B66" cm="1">
+        <f t="array" aca="1" ref="B66" ca="1">_xlfn.XLOOKUP($A66,INDIRECT($A$64),INDIRECT(B$64))</f>
+        <v>0</v>
+      </c>
+      <c r="C66" cm="1">
+        <f t="array" aca="1" ref="C66" ca="1">_xlfn.XLOOKUP($A66,INDIRECT($A$64),INDIRECT(C$64))</f>
+        <v>0</v>
+      </c>
+      <c r="D66" cm="1">
+        <f t="array" aca="1" ref="D66" ca="1">_xlfn.XLOOKUP($A66,INDIRECT($A$64),INDIRECT(D$64))</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4437,16 +4471,16 @@
       <c r="A67" t="s">
         <v>32</v>
       </c>
-      <c r="B67">
-        <f t="shared" si="13"/>
+      <c r="B67" cm="1">
+        <f t="array" aca="1" ref="B67" ca="1">_xlfn.XLOOKUP($A67,INDIRECT($A$64),INDIRECT(B$64))</f>
         <v>-149396.10000000987</v>
       </c>
-      <c r="C67">
-        <f t="shared" si="14"/>
+      <c r="C67" cm="1">
+        <f t="array" aca="1" ref="C67" ca="1">_xlfn.XLOOKUP($A67,INDIRECT($A$64),INDIRECT(C$64))</f>
         <v>-189254.06000000006</v>
       </c>
-      <c r="D67">
-        <f t="shared" si="15"/>
+      <c r="D67" cm="1">
+        <f t="array" aca="1" ref="D67" ca="1">_xlfn.XLOOKUP($A67,INDIRECT($A$64),INDIRECT(D$64))</f>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4454,16 +4488,16 @@
       <c r="A68" t="s">
         <v>38</v>
       </c>
-      <c r="B68">
-        <f t="shared" si="13"/>
+      <c r="B68" cm="1">
+        <f t="array" aca="1" ref="B68" ca="1">_xlfn.XLOOKUP($A68,INDIRECT($A$64),INDIRECT(B$64))</f>
         <v>-12230.810000000056</v>
       </c>
-      <c r="C68">
-        <f t="shared" si="14"/>
+      <c r="C68" cm="1">
+        <f t="array" aca="1" ref="C68" ca="1">_xlfn.XLOOKUP($A68,INDIRECT($A$64),INDIRECT(C$64))</f>
         <v>-45485.580000000075</v>
       </c>
-      <c r="D68">
-        <f t="shared" si="15"/>
+      <c r="D68" cm="1">
+        <f t="array" aca="1" ref="D68" ca="1">_xlfn.XLOOKUP($A68,INDIRECT($A$64),INDIRECT(D$64))</f>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4471,16 +4505,16 @@
       <c r="A69" t="s">
         <v>39</v>
       </c>
-      <c r="B69">
-        <f t="shared" si="13"/>
+      <c r="B69" cm="1">
+        <f t="array" aca="1" ref="B69" ca="1">_xlfn.XLOOKUP($A69,INDIRECT($A$64),INDIRECT(B$64))</f>
         <v>-4950.4699999999721</v>
       </c>
-      <c r="C69">
-        <f t="shared" si="14"/>
+      <c r="C69" cm="1">
+        <f t="array" aca="1" ref="C69" ca="1">_xlfn.XLOOKUP($A69,INDIRECT($A$64),INDIRECT(C$64))</f>
         <v>-8005.7900000010268</v>
       </c>
-      <c r="D69">
-        <f t="shared" si="15"/>
+      <c r="D69" cm="1">
+        <f t="array" aca="1" ref="D69" ca="1">_xlfn.XLOOKUP($A69,INDIRECT($A$64),INDIRECT(D$64))</f>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4488,16 +4522,16 @@
       <c r="A70" t="s">
         <v>55</v>
       </c>
-      <c r="B70">
-        <f t="shared" si="13"/>
+      <c r="B70" cm="1">
+        <f t="array" aca="1" ref="B70" ca="1">_xlfn.XLOOKUP($A70,INDIRECT($A$64),INDIRECT(B$64))</f>
         <v>-184239.79000001028</v>
       </c>
-      <c r="C70">
-        <f t="shared" si="14"/>
+      <c r="C70" cm="1">
+        <f t="array" aca="1" ref="C70" ca="1">_xlfn.XLOOKUP($A70,INDIRECT($A$64),INDIRECT(C$64))</f>
         <v>-133456.33000001032</v>
       </c>
-      <c r="D70">
-        <f t="shared" si="15"/>
+      <c r="D70" cm="1">
+        <f t="array" aca="1" ref="D70" ca="1">_xlfn.XLOOKUP($A70,INDIRECT($A$64),INDIRECT(D$64))</f>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -4529,11 +4563,11 @@
         <v>-36209.630000000005</v>
       </c>
       <c r="C74">
-        <f t="shared" ref="C74:D79" si="16">INDEX($A$1:$P$52,MATCH($A74,$A$1:$A$52,0),MATCH(C$73,$A$1:$P$1,0))</f>
+        <f t="shared" ref="C74:D79" si="13">INDEX($A$1:$P$52,MATCH($A74,$A$1:$A$52,0),MATCH(C$73,$A$1:$P$1,0))</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D74">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -4542,15 +4576,15 @@
         <v>25</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B79" si="17">INDEX($A$1:$P$52,MATCH($A75,$A$1:$A$52,0),MATCH(B$73,$A$1:$P$1,0))</f>
+        <f t="shared" ref="B75:B79" si="14">INDEX($A$1:$P$52,MATCH($A75,$A$1:$A$52,0),MATCH(B$73,$A$1:$P$1,0))</f>
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4559,15 +4593,15 @@
         <v>32</v>
       </c>
       <c r="B76">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C76">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D76">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4576,15 +4610,15 @@
         <v>38</v>
       </c>
       <c r="B77">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C77">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D77">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4593,15 +4627,15 @@
         <v>39</v>
       </c>
       <c r="B78">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C78">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D78">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4610,15 +4644,15 @@
         <v>55</v>
       </c>
       <c r="B79">
-        <f t="shared" si="17"/>
+        <f t="shared" si="14"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C79">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D79">
-        <f t="shared" si="16"/>
+        <f t="shared" si="13"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -4661,11 +4695,11 @@
         <v>74</v>
       </c>
       <c r="B85" s="6">
-        <f t="shared" ref="B85:C86" si="18">INDEX($A$1:$P$52,MATCH($A$83,$A$1:$A$52,0),MATCH(_xlfn.CONCAT($A85,"_",B$83),$A$1:$P$1,0))</f>
+        <f t="shared" ref="B85:C86" si="15">INDEX($A$1:$P$52,MATCH($A$83,$A$1:$A$52,0),MATCH(_xlfn.CONCAT($A85,"_",B$83),$A$1:$P$1,0))</f>
         <v>859100</v>
       </c>
       <c r="C85" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>859100</v>
       </c>
     </row>
@@ -4674,11 +4708,11 @@
         <v>75</v>
       </c>
       <c r="B86" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>843200</v>
       </c>
       <c r="C86" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="15"/>
         <v>843200</v>
       </c>
     </row>
@@ -4727,24 +4761,88 @@
       <c r="A91" t="s">
         <v>73</v>
       </c>
-      <c r="E91" s="5"/>
-      <c r="G91" s="5"/>
+      <c r="B91" t="str" cm="1">
+        <f t="array" aca="1" ref="B91" ca="1">_xlfn.XLOOKUP(B$89,INDIRECT($A91&amp;"_rank"),Department)</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="C91" s="5">
+        <f ca="1">INDEX($A$1:$P$52,MATCH(B91,INDIRECT(B$90),0),MATCH(_xlfn.CONCAT($A91,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-0.15235918433091292</v>
+      </c>
+      <c r="D91" t="str" cm="1">
+        <f t="array" aca="1" ref="D91" ca="1">_xlfn.XLOOKUP(D$89,INDIRECT($A91&amp;"_rank"),Department)</f>
+        <v>Circuit Court Clerk</v>
+      </c>
+      <c r="E91" s="5">
+        <f ca="1">INDEX($A$1:$P$52,MATCH(D91,INDIRECT(D$90),0),MATCH(_xlfn.CONCAT($A91,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-0.11502817362571344</v>
+      </c>
+      <c r="F91" t="str" cm="1">
+        <f t="array" aca="1" ref="F91" ca="1">_xlfn.XLOOKUP(F$89,INDIRECT($A91&amp;"_rank"),Department)</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="G91" s="5">
+        <f ca="1">INDEX($A$1:$P$52,MATCH(F91,INDIRECT(F$90),0),MATCH(_xlfn.CONCAT($A91,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-9.5782760864849215E-2</v>
+      </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>74</v>
       </c>
-      <c r="C92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="G92" s="5"/>
+      <c r="B92" t="str" cm="1">
+        <f t="array" aca="1" ref="B92" ca="1">_xlfn.XLOOKUP(B$89,INDIRECT($A92&amp;"_rank"),Department)</f>
+        <v>Metropolitan Clerk</v>
+      </c>
+      <c r="C92" s="5">
+        <f t="shared" ref="C92:E93" ca="1" si="16">INDEX($A$1:$P$52,MATCH(B92,INDIRECT(B$90),0),MATCH(_xlfn.CONCAT($A92,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-0.17551246244575608</v>
+      </c>
+      <c r="D92" t="str" cm="1">
+        <f t="array" aca="1" ref="D92" ca="1">_xlfn.XLOOKUP(D$89,INDIRECT($A92&amp;"_rank"),Department)</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="E92" s="5">
+        <f t="shared" ca="1" si="16"/>
+        <v>-0.17103239309050916</v>
+      </c>
+      <c r="F92" t="str" cm="1">
+        <f t="array" aca="1" ref="F92" ca="1">_xlfn.XLOOKUP(F$89,INDIRECT($A92&amp;"_rank"),Department)</f>
+        <v>Office of Family Safety</v>
+      </c>
+      <c r="G92" s="5">
+        <f t="shared" ref="G92" ca="1" si="17">INDEX($A$1:$P$52,MATCH(F92,INDIRECT(F$90),0),MATCH(_xlfn.CONCAT($A92,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-0.13918241656366656</v>
+      </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>75</v>
       </c>
-      <c r="C93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="G93" s="5"/>
+      <c r="B93" t="str" cm="1">
+        <f t="array" aca="1" ref="B93" ca="1">_xlfn.XLOOKUP(B$89,INDIRECT($A93&amp;"_rank"),Department)</f>
+        <v>Community Oversight Board</v>
+      </c>
+      <c r="C93" s="5">
+        <f t="shared" ca="1" si="16"/>
+        <v>-0.82994157333333329</v>
+      </c>
+      <c r="D93" t="str" cm="1">
+        <f t="array" aca="1" ref="D93" ca="1">_xlfn.XLOOKUP(D$89,INDIRECT($A93&amp;"_rank"),Department)</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="E93" s="5">
+        <f t="shared" ref="E93" ca="1" si="18">INDEX($A$1:$P$52,MATCH(D93,INDIRECT(D$90),0),MATCH(_xlfn.CONCAT($A93,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-0.15295680364719175</v>
+      </c>
+      <c r="F93" t="str" cm="1">
+        <f t="array" aca="1" ref="F93" ca="1">_xlfn.XLOOKUP(F$89,INDIRECT($A93&amp;"_rank"),Department)</f>
+        <v>Election Commission</v>
+      </c>
+      <c r="G93" s="5">
+        <f t="shared" ref="G93" ca="1" si="19">INDEX($A$1:$P$52,MATCH(F93,INDIRECT(F$90),0),MATCH(_xlfn.CONCAT($A93,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-0.12882667147667154</v>
+      </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
@@ -4791,31 +4889,94 @@
       <c r="A98" t="s">
         <v>73</v>
       </c>
-      <c r="C98" s="4"/>
-      <c r="E98" s="4"/>
-      <c r="G98" s="4"/>
+      <c r="B98" t="str">
+        <f ca="1">INDEX($A$1:$P$52,MATCH(B$96,INDIRECT($A98&amp;"_rank"),0),MATCH($B$97,$A$1:$P$1,0))</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="C98" s="4">
+        <f ca="1">INDEX($A$1:$P$52,MATCH(B98,Department,0),MATCH(_xlfn.CONCAT($A98,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-0.15235918433091292</v>
+      </c>
+      <c r="D98" t="str">
+        <f ca="1">INDEX($A$1:$P$52,MATCH(D$96,INDIRECT($A98&amp;"_rank"),0),MATCH($B$97,$A$1:$P$1,0))</f>
+        <v>Circuit Court Clerk</v>
+      </c>
+      <c r="E98" s="4">
+        <f ca="1">INDEX($A$1:$P$52,MATCH(D98,Department,0),MATCH(_xlfn.CONCAT($A98,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-0.11502817362571344</v>
+      </c>
+      <c r="F98" t="str">
+        <f ca="1">INDEX($A$1:$P$52,MATCH(F$96,INDIRECT($A98&amp;"_rank"),0),MATCH($B$97,$A$1:$P$1,0))</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="G98" s="4">
+        <f ca="1">INDEX($A$1:$P$52,MATCH(F98,Department,0),MATCH(_xlfn.CONCAT($A98,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-9.5782760864849215E-2</v>
+      </c>
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>74</v>
       </c>
-      <c r="C99" s="4"/>
-      <c r="E99" s="4"/>
-      <c r="G99" s="4"/>
+      <c r="B99" t="str">
+        <f t="shared" ref="B99:F100" ca="1" si="20">INDEX($A$1:$P$52,MATCH(B$96,INDIRECT($A99&amp;"_rank"),0),MATCH($B$97,$A$1:$P$1,0))</f>
+        <v>Metropolitan Clerk</v>
+      </c>
+      <c r="C99" s="4">
+        <f ca="1">INDEX($A$1:$P$52,MATCH(B99,Department,0),MATCH(_xlfn.CONCAT($A99,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-0.17551246244575608</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>Internal Audit</v>
+      </c>
+      <c r="E99" s="4">
+        <f ca="1">INDEX($A$1:$P$52,MATCH(D99,Department,0),MATCH(_xlfn.CONCAT($A99,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-0.17103239309050916</v>
+      </c>
+      <c r="F99" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>Office of Family Safety</v>
+      </c>
+      <c r="G99" s="4">
+        <f ca="1">INDEX($A$1:$P$52,MATCH(F99,Department,0),MATCH(_xlfn.CONCAT($A99,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-0.13918241656366656</v>
+      </c>
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>75</v>
       </c>
-      <c r="C100" s="4"/>
-      <c r="E100" s="4"/>
-      <c r="G100" s="4"/>
+      <c r="B100" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>Community Oversight Board</v>
+      </c>
+      <c r="C100" s="4">
+        <f ca="1">INDEX($A$1:$P$52,MATCH(B100,Department,0),MATCH(_xlfn.CONCAT($A100,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-0.82994157333333329</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="E100" s="4">
+        <f ca="1">INDEX($A$1:$P$52,MATCH(D100,Department,0),MATCH(_xlfn.CONCAT($A100,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-0.15295680364719175</v>
+      </c>
+      <c r="F100" t="str">
+        <f t="shared" ca="1" si="20"/>
+        <v>Election Commission</v>
+      </c>
+      <c r="G100" s="4">
+        <f ca="1">INDEX($A$1:$P$52,MATCH(F100,Department,0),MATCH(_xlfn.CONCAT($A100,"_diff_pct"),$A$1:$P$1,0))</f>
+        <v>-0.12882667147667154</v>
+      </c>
       <c r="I100" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Index is a cruel and fickle mistress.
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sirli\Documents\DA13\Excel\lookups-exercise-ryanphenderson\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC34943D-E97A-477C-AFE6-B42CF62CE3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A616F3-E61B-4108-B900-96C8746DEFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1212,7 +1212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
@@ -4307,10 +4307,6 @@
       <c r="D55" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G55">
-        <f>COLUMN(C55)</f>
-        <v>3</v>
-      </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
@@ -4438,15 +4434,15 @@
         <v>24</v>
       </c>
       <c r="B65" cm="1">
-        <f t="array" aca="1" ref="B65" ca="1">_xlfn.XLOOKUP($A65,INDIRECT($A$64),INDIRECT(B$64))</f>
+        <f t="array" ref="B65">_xlfn.XLOOKUP($A65,Department,INDEX($A$1:$P$52,,MATCH(B$64,$A$1:$P$1,0)))</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C65" cm="1">
-        <f t="array" aca="1" ref="C65" ca="1">_xlfn.XLOOKUP($A65,INDIRECT($A$64),INDIRECT(C$64))</f>
+        <f t="array" ref="C65">_xlfn.XLOOKUP($A65,Department,INDEX($A$1:$P$52,,MATCH(C$64,$A$1:$P$1,0)))</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D65" cm="1">
-        <f t="array" aca="1" ref="D65" ca="1">_xlfn.XLOOKUP($A65,INDIRECT($A$64),INDIRECT(D$64))</f>
+        <f t="array" ref="D65">_xlfn.XLOOKUP($A65,Department,INDEX($A$1:$P$52,,MATCH(D$64,$A$1:$P$1,0)))</f>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -4455,15 +4451,15 @@
         <v>25</v>
       </c>
       <c r="B66" cm="1">
-        <f t="array" aca="1" ref="B66" ca="1">_xlfn.XLOOKUP($A66,INDIRECT($A$64),INDIRECT(B$64))</f>
+        <f t="array" ref="B66">_xlfn.XLOOKUP($A66,Department,INDEX($A$1:$P$52,,MATCH(B$64,$A$1:$P$1,0)))</f>
         <v>0</v>
       </c>
       <c r="C66" cm="1">
-        <f t="array" aca="1" ref="C66" ca="1">_xlfn.XLOOKUP($A66,INDIRECT($A$64),INDIRECT(C$64))</f>
+        <f t="array" ref="C66">_xlfn.XLOOKUP($A66,Department,INDEX($A$1:$P$52,,MATCH(C$64,$A$1:$P$1,0)))</f>
         <v>0</v>
       </c>
       <c r="D66" cm="1">
-        <f t="array" aca="1" ref="D66" ca="1">_xlfn.XLOOKUP($A66,INDIRECT($A$64),INDIRECT(D$64))</f>
+        <f t="array" ref="D66">_xlfn.XLOOKUP($A66,Department,INDEX($A$1:$P$52,,MATCH(D$64,$A$1:$P$1,0)))</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4472,15 +4468,15 @@
         <v>32</v>
       </c>
       <c r="B67" cm="1">
-        <f t="array" aca="1" ref="B67" ca="1">_xlfn.XLOOKUP($A67,INDIRECT($A$64),INDIRECT(B$64))</f>
+        <f t="array" ref="B67">_xlfn.XLOOKUP($A67,Department,INDEX($A$1:$P$52,,MATCH(B$64,$A$1:$P$1,0)))</f>
         <v>-149396.10000000987</v>
       </c>
       <c r="C67" cm="1">
-        <f t="array" aca="1" ref="C67" ca="1">_xlfn.XLOOKUP($A67,INDIRECT($A$64),INDIRECT(C$64))</f>
+        <f t="array" ref="C67">_xlfn.XLOOKUP($A67,Department,INDEX($A$1:$P$52,,MATCH(C$64,$A$1:$P$1,0)))</f>
         <v>-189254.06000000006</v>
       </c>
       <c r="D67" cm="1">
-        <f t="array" aca="1" ref="D67" ca="1">_xlfn.XLOOKUP($A67,INDIRECT($A$64),INDIRECT(D$64))</f>
+        <f t="array" ref="D67">_xlfn.XLOOKUP($A67,Department,INDEX($A$1:$P$52,,MATCH(D$64,$A$1:$P$1,0)))</f>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4489,15 +4485,15 @@
         <v>38</v>
       </c>
       <c r="B68" cm="1">
-        <f t="array" aca="1" ref="B68" ca="1">_xlfn.XLOOKUP($A68,INDIRECT($A$64),INDIRECT(B$64))</f>
+        <f t="array" ref="B68">_xlfn.XLOOKUP($A68,Department,INDEX($A$1:$P$52,,MATCH(B$64,$A$1:$P$1,0)))</f>
         <v>-12230.810000000056</v>
       </c>
       <c r="C68" cm="1">
-        <f t="array" aca="1" ref="C68" ca="1">_xlfn.XLOOKUP($A68,INDIRECT($A$64),INDIRECT(C$64))</f>
+        <f t="array" ref="C68">_xlfn.XLOOKUP($A68,Department,INDEX($A$1:$P$52,,MATCH(C$64,$A$1:$P$1,0)))</f>
         <v>-45485.580000000075</v>
       </c>
       <c r="D68" cm="1">
-        <f t="array" aca="1" ref="D68" ca="1">_xlfn.XLOOKUP($A68,INDIRECT($A$64),INDIRECT(D$64))</f>
+        <f t="array" ref="D68">_xlfn.XLOOKUP($A68,Department,INDEX($A$1:$P$52,,MATCH(D$64,$A$1:$P$1,0)))</f>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4506,15 +4502,15 @@
         <v>39</v>
       </c>
       <c r="B69" cm="1">
-        <f t="array" aca="1" ref="B69" ca="1">_xlfn.XLOOKUP($A69,INDIRECT($A$64),INDIRECT(B$64))</f>
+        <f t="array" ref="B69">_xlfn.XLOOKUP($A69,Department,INDEX($A$1:$P$52,,MATCH(B$64,$A$1:$P$1,0)))</f>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C69" cm="1">
-        <f t="array" aca="1" ref="C69" ca="1">_xlfn.XLOOKUP($A69,INDIRECT($A$64),INDIRECT(C$64))</f>
+        <f t="array" ref="C69">_xlfn.XLOOKUP($A69,Department,INDEX($A$1:$P$52,,MATCH(C$64,$A$1:$P$1,0)))</f>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D69" cm="1">
-        <f t="array" aca="1" ref="D69" ca="1">_xlfn.XLOOKUP($A69,INDIRECT($A$64),INDIRECT(D$64))</f>
+        <f t="array" ref="D69">_xlfn.XLOOKUP($A69,Department,INDEX($A$1:$P$52,,MATCH(D$64,$A$1:$P$1,0)))</f>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4523,15 +4519,15 @@
         <v>55</v>
       </c>
       <c r="B70" cm="1">
-        <f t="array" aca="1" ref="B70" ca="1">_xlfn.XLOOKUP($A70,INDIRECT($A$64),INDIRECT(B$64))</f>
+        <f t="array" ref="B70">_xlfn.XLOOKUP($A70,Department,INDEX($A$1:$P$52,,MATCH(B$64,$A$1:$P$1,0)))</f>
         <v>-184239.79000001028</v>
       </c>
       <c r="C70" cm="1">
-        <f t="array" aca="1" ref="C70" ca="1">_xlfn.XLOOKUP($A70,INDIRECT($A$64),INDIRECT(C$64))</f>
+        <f t="array" ref="C70">_xlfn.XLOOKUP($A70,Department,INDEX($A$1:$P$52,,MATCH(C$64,$A$1:$P$1,0)))</f>
         <v>-133456.33000001032</v>
       </c>
       <c r="D70" cm="1">
-        <f t="array" aca="1" ref="D70" ca="1">_xlfn.XLOOKUP($A70,INDIRECT($A$64),INDIRECT(D$64))</f>
+        <f t="array" ref="D70">_xlfn.XLOOKUP($A70,Department,INDEX($A$1:$P$52,,MATCH(D$64,$A$1:$P$1,0)))</f>
         <v>-82077.349999999627</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Complete, with the chart this time!
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sirli\Documents\DA13\Excel\lookups-exercise-ryanphenderson\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A616F3-E61B-4108-B900-96C8746DEFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0360EC7-4040-4826-84B0-4E58BF1AC905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -913,6 +913,1060 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>metro_budget!$A$83</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>Criminal Justice Planning</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$B$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Budget</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$B$84:$B$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>512000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>530500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>526200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3A01-4D19-A8C9-BBDA6425DF0D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$C$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$C$84:$C$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>505017.37</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>524402.98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>504989.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3A01-4D19-A8C9-BBDA6425DF0D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="-25"/>
+        <c:axId val="19466608"/>
+        <c:axId val="8495680"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="19466608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="8495680"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="8495680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="19466608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A31CE82-C4F2-E95B-D19B-06618FC1F2E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -1212,8 +2266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,7 +2884,7 @@
         <v>0</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(B11=0,"N/A",_xlfn.RANK.EQ(E11,$E$2:$E$52,1))</f>
         <v>N/A</v>
       </c>
       <c r="G11">
@@ -4664,7 +5718,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>71</v>
@@ -4679,11 +5733,11 @@
       </c>
       <c r="B84" s="6">
         <f>INDEX($A$1:$P$52,MATCH($A$83,$A$1:$A$52,0),MATCH(_xlfn.CONCAT($A84,"_",B$83),$A$1:$P$1,0))</f>
-        <v>832600</v>
+        <v>512000</v>
       </c>
       <c r="C84" s="6">
         <f>INDEX($A$1:$P$52,MATCH($A$83,$A$1:$A$52,0),MATCH(_xlfn.CONCAT($A84,"_",C$83),$A$1:$P$1,0))</f>
-        <v>832600</v>
+        <v>505017.37</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -4692,11 +5746,11 @@
       </c>
       <c r="B85" s="6">
         <f t="shared" ref="B85:C86" si="15">INDEX($A$1:$P$52,MATCH($A$83,$A$1:$A$52,0),MATCH(_xlfn.CONCAT($A85,"_",B$83),$A$1:$P$1,0))</f>
-        <v>859100</v>
+        <v>530500</v>
       </c>
       <c r="C85" s="6">
         <f t="shared" si="15"/>
-        <v>859100</v>
+        <v>524402.98</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -4705,11 +5759,11 @@
       </c>
       <c r="B86" s="6">
         <f t="shared" si="15"/>
-        <v>843200</v>
+        <v>526200</v>
       </c>
       <c r="C86" s="6">
         <f t="shared" si="15"/>
-        <v>843200</v>
+        <v>504989.88</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -4972,13 +6026,14 @@
       <c r="I100" s="4"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Signed, Sealed, Delivered: It's done.
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sirli\Documents\DA13\Excel\lookups-exercise-ryanphenderson\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0360EC7-4040-4826-84B0-4E58BF1AC905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB7AA83-D520-47AE-BB71-2596451EB907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1931,15 +1931,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:colOff>9525</xdr:colOff>
       <xdr:row>70</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>88</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2267,7 +2267,7 @@
   <dimension ref="A1:P100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="H64" sqref="H64"/>
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>